<commit_message>
agregado de etiqueta 312-HE-BRAZUELO MUNON 8M - jabat
</commit_message>
<xml_diff>
--- a/jabad def.xlsx
+++ b/jabad def.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5A4483-D46E-4E4B-8103-38ED379A5E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E838A65E-1C81-47AE-B19D-1E653F975CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -902,7 +902,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -977,18 +977,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
@@ -998,9 +989,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1030,42 +1018,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1116,6 +1068,45 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1402,7 +1393,7 @@
   <dimension ref="A1:N41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1422,60 +1413,60 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="62" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1"/>
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="52" t="s">
+      <c r="D2" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="52" t="s">
+      <c r="E2" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="50" t="s">
+      <c r="H2" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="54" t="s">
+      <c r="I2" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="44" t="s">
+      <c r="J2" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="46" t="s">
+      <c r="K2" s="60" t="s">
         <v>7</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="57" t="s">
+      <c r="N2" s="41" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="49"/>
+      <c r="A3" s="63"/>
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
       <c r="F3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="51"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="47"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="61"/>
       <c r="L3" s="5" t="s">
         <v>13</v>
       </c>
@@ -1511,7 +1502,7 @@
       <c r="J4" s="11">
         <v>101861</v>
       </c>
-      <c r="K4" s="58" t="s">
+      <c r="K4" s="42" t="s">
         <v>21</v>
       </c>
       <c r="L4" s="12" t="s">
@@ -1549,7 +1540,7 @@
       <c r="J5" s="11">
         <v>101862</v>
       </c>
-      <c r="K5" s="59" t="s">
+      <c r="K5" s="43" t="s">
         <v>21</v>
       </c>
       <c r="L5" s="12" t="s">
@@ -1585,14 +1576,14 @@
       <c r="J6" s="11">
         <v>101865</v>
       </c>
-      <c r="K6" s="59" t="s">
+      <c r="K6" s="43" t="s">
         <v>33</v>
       </c>
       <c r="L6" s="12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="171" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="57" x14ac:dyDescent="0.25">
       <c r="A7" s="17">
         <v>2</v>
       </c>
@@ -1623,7 +1614,7 @@
       <c r="J7" s="11">
         <v>102531</v>
       </c>
-      <c r="K7" s="60" t="s">
+      <c r="K7" s="44" t="s">
         <v>39</v>
       </c>
       <c r="L7" s="12" t="s">
@@ -1652,10 +1643,10 @@
       </c>
       <c r="I8" s="20"/>
       <c r="J8" s="20"/>
-      <c r="K8" s="61"/>
+      <c r="K8" s="45"/>
       <c r="L8" s="20"/>
     </row>
-    <row r="9" spans="1:14" ht="114" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="57" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>41</v>
       </c>
@@ -1686,14 +1677,14 @@
       <c r="J9" s="11">
         <v>102533</v>
       </c>
-      <c r="K9" s="60" t="s">
+      <c r="K9" s="44" t="s">
         <v>46</v>
       </c>
       <c r="L9" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="114" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="57" x14ac:dyDescent="0.25">
       <c r="A10" s="22">
         <v>22</v>
       </c>
@@ -1724,14 +1715,14 @@
       <c r="J10" s="11">
         <v>102534</v>
       </c>
-      <c r="K10" s="60" t="s">
+      <c r="K10" s="44" t="s">
         <v>51</v>
       </c>
       <c r="L10" s="12" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="114" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="57" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>53</v>
       </c>
@@ -1762,14 +1753,14 @@
       <c r="J11" s="11">
         <v>103521</v>
       </c>
-      <c r="K11" s="60" t="s">
+      <c r="K11" s="44" t="s">
         <v>58</v>
       </c>
       <c r="L11" s="12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="114" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="57" x14ac:dyDescent="0.25">
       <c r="A12" s="22">
         <v>33</v>
       </c>
@@ -1800,14 +1791,14 @@
       <c r="J12" s="11">
         <v>103522</v>
       </c>
-      <c r="K12" s="60" t="s">
+      <c r="K12" s="44" t="s">
         <v>62</v>
       </c>
       <c r="L12" s="12" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="114" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="57" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>63</v>
       </c>
@@ -1838,14 +1829,14 @@
       <c r="J13" s="11">
         <v>103523</v>
       </c>
-      <c r="K13" s="60" t="s">
+      <c r="K13" s="44" t="s">
         <v>69</v>
       </c>
       <c r="L13" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="114" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="57" x14ac:dyDescent="0.25">
       <c r="A14" s="22">
         <v>3</v>
       </c>
@@ -1876,14 +1867,14 @@
       <c r="J14" s="11">
         <v>103524</v>
       </c>
-      <c r="K14" s="60" t="s">
+      <c r="K14" s="44" t="s">
         <v>73</v>
       </c>
       <c r="L14" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="114" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="57" x14ac:dyDescent="0.25">
       <c r="A15" s="22">
         <v>44</v>
       </c>
@@ -1914,14 +1905,14 @@
       <c r="J15" s="11">
         <v>104521</v>
       </c>
-      <c r="K15" s="60" t="s">
+      <c r="K15" s="44" t="s">
         <v>78</v>
       </c>
       <c r="L15" s="12" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="114" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="57" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>80</v>
       </c>
@@ -1952,14 +1943,14 @@
       <c r="J16" s="11">
         <v>104522</v>
       </c>
-      <c r="K16" s="60" t="s">
+      <c r="K16" s="44" t="s">
         <v>85</v>
       </c>
       <c r="L16" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="114" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="57" x14ac:dyDescent="0.25">
       <c r="A17" s="22">
         <v>4</v>
       </c>
@@ -1990,14 +1981,14 @@
       <c r="J17" s="11">
         <v>104523</v>
       </c>
-      <c r="K17" s="60" t="s">
+      <c r="K17" s="44" t="s">
         <v>90</v>
       </c>
       <c r="L17" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="171" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="57" x14ac:dyDescent="0.25">
       <c r="A18" s="22">
         <v>55</v>
       </c>
@@ -2028,7 +2019,7 @@
       <c r="J18" s="11">
         <v>105521</v>
       </c>
-      <c r="K18" s="60" t="s">
+      <c r="K18" s="44" t="s">
         <v>95</v>
       </c>
       <c r="L18" s="12" t="s">
@@ -2064,7 +2055,7 @@
       <c r="J19" s="11">
         <v>105522</v>
       </c>
-      <c r="K19" s="62" t="s">
+      <c r="K19" s="46" t="s">
         <v>100</v>
       </c>
       <c r="L19" s="12" t="s">
@@ -2100,7 +2091,7 @@
       <c r="J20" s="11">
         <v>106521</v>
       </c>
-      <c r="K20" s="62" t="s">
+      <c r="K20" s="46" t="s">
         <v>104</v>
       </c>
       <c r="L20" s="12" t="s">
@@ -2136,7 +2127,7 @@
       <c r="J21" s="11">
         <v>107521</v>
       </c>
-      <c r="K21" s="62" t="s">
+      <c r="K21" s="46" t="s">
         <v>109</v>
       </c>
       <c r="L21" s="12" t="s">
@@ -2174,7 +2165,7 @@
       <c r="J22" s="11">
         <v>108521</v>
       </c>
-      <c r="K22" s="62" t="s">
+      <c r="K22" s="46" t="s">
         <v>115</v>
       </c>
       <c r="L22" s="12" t="s">
@@ -2182,83 +2173,83 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="56" t="s">
+      <c r="A23" s="40" t="s">
         <v>116</v>
       </c>
-      <c r="B23" s="68" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="68" t="s">
+      <c r="B23" s="52" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="52" t="s">
         <v>117</v>
       </c>
-      <c r="D23" s="69"/>
-      <c r="E23" s="70"/>
-      <c r="F23" s="68" t="s">
+      <c r="D23" s="53"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="G23" s="68" t="s">
-        <v>26</v>
-      </c>
-      <c r="H23" s="68" t="s">
+      <c r="G23" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="H23" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="I23" s="71">
+      <c r="I23" s="55">
         <v>7290019570820</v>
       </c>
-      <c r="J23" s="72">
+      <c r="J23" s="56">
         <v>108523</v>
       </c>
-      <c r="K23" s="67" t="s">
+      <c r="K23" s="51" t="s">
         <v>119</v>
       </c>
-      <c r="L23" s="73" t="s">
+      <c r="L23" s="57" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="57" x14ac:dyDescent="0.25">
-      <c r="A24" s="26" t="s">
+    <row r="24" spans="1:12" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="B24" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="27" t="s">
+      <c r="B24" s="70" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="52" t="s">
         <v>121</v>
       </c>
-      <c r="D24" s="28"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="27" t="s">
+      <c r="D24" s="53"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="52" t="s">
         <v>122</v>
       </c>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27" t="s">
+      <c r="G24" s="52"/>
+      <c r="H24" s="52" t="s">
         <v>123</v>
       </c>
-      <c r="I24" s="30">
+      <c r="I24" s="55">
         <v>7290019570820</v>
       </c>
-      <c r="J24" s="31">
+      <c r="J24" s="56">
         <v>188521</v>
       </c>
-      <c r="K24" s="63" t="s">
+      <c r="K24" s="51" t="s">
         <v>124</v>
       </c>
-      <c r="L24" s="32" t="s">
+      <c r="L24" s="57" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="57" x14ac:dyDescent="0.25">
-      <c r="A25" s="56" t="s">
+      <c r="A25" s="40" t="s">
         <v>125</v>
       </c>
-      <c r="B25" s="34" t="s">
+      <c r="B25" s="30" t="s">
         <v>24</v>
       </c>
       <c r="C25" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="D25" s="35"/>
-      <c r="E25" s="36" t="s">
+      <c r="D25" s="31"/>
+      <c r="E25" s="32" t="s">
         <v>127</v>
       </c>
       <c r="F25" s="14" t="s">
@@ -2270,13 +2261,13 @@
       <c r="H25" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="I25" s="37">
+      <c r="I25" s="33">
         <v>7290019570813</v>
       </c>
       <c r="J25" s="11">
         <v>108522</v>
       </c>
-      <c r="K25" s="64" t="s">
+      <c r="K25" s="48" t="s">
         <v>129</v>
       </c>
       <c r="L25" s="12" t="s">
@@ -2284,19 +2275,19 @@
       </c>
     </row>
     <row r="26" spans="1:12" ht="57" x14ac:dyDescent="0.25">
-      <c r="A26" s="38" t="s">
+      <c r="A26" s="34" t="s">
         <v>130</v>
       </c>
-      <c r="B26" s="34" t="s">
+      <c r="B26" s="30" t="s">
         <v>24</v>
       </c>
       <c r="C26" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="D26" s="39" t="s">
+      <c r="D26" s="35" t="s">
         <v>132</v>
       </c>
-      <c r="E26" s="36" t="s">
+      <c r="E26" s="32" t="s">
         <v>133</v>
       </c>
       <c r="F26" s="14" t="s">
@@ -2308,20 +2299,20 @@
       <c r="H26" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="I26" s="37">
+      <c r="I26" s="33">
         <v>7290019570806</v>
       </c>
       <c r="J26" s="11">
         <v>110531</v>
       </c>
-      <c r="K26" s="65" t="s">
+      <c r="K26" s="49" t="s">
         <v>135</v>
       </c>
       <c r="L26" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="114" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="57" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
         <v>136</v>
       </c>
@@ -2352,14 +2343,14 @@
       <c r="J27" s="11">
         <v>110532</v>
       </c>
-      <c r="K27" s="60" t="s">
+      <c r="K27" s="44" t="s">
         <v>140</v>
       </c>
       <c r="L27" s="12" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="114" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="57" x14ac:dyDescent="0.25">
       <c r="A28" s="22">
         <v>10</v>
       </c>
@@ -2390,7 +2381,7 @@
       <c r="J28" s="11">
         <v>110533</v>
       </c>
-      <c r="K28" s="60" t="s">
+      <c r="K28" s="44" t="s">
         <v>146</v>
       </c>
       <c r="L28" s="12" t="s">
@@ -2426,48 +2417,48 @@
       <c r="J29" s="11">
         <v>170521</v>
       </c>
-      <c r="K29" s="62" t="s">
+      <c r="K29" s="46" t="s">
         <v>151</v>
       </c>
       <c r="L29" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="57" x14ac:dyDescent="0.25">
-      <c r="A30" s="40" t="s">
+    <row r="30" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A30" s="36" t="s">
         <v>152</v>
       </c>
-      <c r="B30" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="C30" s="27" t="s">
+      <c r="B30" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="26" t="s">
         <v>153</v>
       </c>
-      <c r="D30" s="41"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="27" t="s">
+      <c r="D30" s="37"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="G30" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="H30" s="43" t="s">
+      <c r="G30" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="H30" s="39" t="s">
         <v>154</v>
       </c>
-      <c r="I30" s="30">
+      <c r="I30" s="27">
         <v>7290019570783</v>
       </c>
-      <c r="J30" s="31">
+      <c r="J30" s="28">
         <v>170522</v>
       </c>
-      <c r="K30" s="63" t="s">
+      <c r="K30" s="47" t="s">
         <v>155</v>
       </c>
-      <c r="L30" s="32" t="s">
+      <c r="L30" s="29" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="228" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="114" x14ac:dyDescent="0.25">
       <c r="A31" s="22">
         <v>99</v>
       </c>
@@ -2498,7 +2489,7 @@
       <c r="J31" s="11">
         <v>109521</v>
       </c>
-      <c r="K31" s="66" t="s">
+      <c r="K31" s="50" t="s">
         <v>160</v>
       </c>
       <c r="L31" s="12" t="s">
@@ -2534,7 +2525,7 @@
       <c r="J32" s="11">
         <v>109522</v>
       </c>
-      <c r="K32" s="62" t="s">
+      <c r="K32" s="46" t="s">
         <v>164</v>
       </c>
       <c r="L32" s="12" t="s">
@@ -2570,7 +2561,7 @@
       <c r="J33" s="11">
         <v>109523</v>
       </c>
-      <c r="K33" s="62" t="s">
+      <c r="K33" s="46" t="s">
         <v>168</v>
       </c>
       <c r="L33" s="12" t="s">
@@ -2604,7 +2595,7 @@
       <c r="J34" s="11">
         <v>157521</v>
       </c>
-      <c r="K34" s="62" t="s">
+      <c r="K34" s="46" t="s">
         <v>172</v>
       </c>
       <c r="L34" s="12" t="s">
@@ -2640,7 +2631,7 @@
       <c r="J35" s="11">
         <v>109524</v>
       </c>
-      <c r="K35" s="62" t="s">
+      <c r="K35" s="46" t="s">
         <v>177</v>
       </c>
       <c r="L35" s="12" t="s">
@@ -2672,14 +2663,14 @@
       <c r="J36" s="11">
         <v>109525</v>
       </c>
-      <c r="K36" s="64" t="s">
+      <c r="K36" s="48" t="s">
         <v>179</v>
       </c>
       <c r="L36" s="12" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="114" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" ht="57" x14ac:dyDescent="0.25">
       <c r="A37" s="17"/>
       <c r="B37" s="14" t="s">
         <v>24</v>
@@ -2706,7 +2697,7 @@
       <c r="J37" s="11">
         <v>155521</v>
       </c>
-      <c r="K37" s="66" t="s">
+      <c r="K37" s="50" t="s">
         <v>185</v>
       </c>
       <c r="L37" s="12" t="s">
@@ -2740,7 +2731,7 @@
       <c r="J38" s="11">
         <v>153521</v>
       </c>
-      <c r="K38" s="62" t="s">
+      <c r="K38" s="46" t="s">
         <v>189</v>
       </c>
       <c r="L38" s="12" t="s">
@@ -2774,14 +2765,14 @@
       <c r="J39" s="11">
         <v>150521</v>
       </c>
-      <c r="K39" s="62" t="s">
+      <c r="K39" s="46" t="s">
         <v>193</v>
       </c>
       <c r="L39" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="114" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="57" x14ac:dyDescent="0.25">
       <c r="A40" s="17"/>
       <c r="B40" s="14" t="s">
         <v>24</v>
@@ -2810,7 +2801,7 @@
       <c r="J40" s="11">
         <v>151521</v>
       </c>
-      <c r="K40" s="60" t="s">
+      <c r="K40" s="44" t="s">
         <v>196</v>
       </c>
       <c r="L40" s="12" t="s">
@@ -2846,7 +2837,7 @@
       <c r="J41" s="11">
         <v>156521</v>
       </c>
-      <c r="K41" s="64" t="s">
+      <c r="K41" s="48" t="s">
         <v>200</v>
       </c>
       <c r="L41" s="12" t="s">

</xml_diff>

<commit_message>
agregado de etiqueta 313-HE-TAPABIFELONJAS 17L - jabat
</commit_message>
<xml_diff>
--- a/jabad def.xlsx
+++ b/jabad def.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E838A65E-1C81-47AE-B19D-1E653F975CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07303E88-A29C-40BA-9075-6ADF202B32FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -705,7 +705,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -733,12 +733,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -902,7 +896,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -977,18 +971,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1007,22 +989,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" readingOrder="2"/>
     </xf>
@@ -1036,38 +1006,38 @@
     <xf numFmtId="1" fontId="6" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" readingOrder="2"/>
     </xf>
+    <xf numFmtId="1" fontId="6" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
     <xf numFmtId="1" fontId="6" fillId="6" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" readingOrder="2"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="7" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1105,8 +1075,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1392,8 +1371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1413,60 +1392,60 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="54" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1"/>
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="66" t="s">
+      <c r="D2" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="66" t="s">
+      <c r="E2" s="58" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="64" t="s">
+      <c r="H2" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="68" t="s">
+      <c r="I2" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="58" t="s">
+      <c r="J2" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="60" t="s">
+      <c r="K2" s="52" t="s">
         <v>7</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="41" t="s">
+      <c r="N2" s="33" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="63"/>
+      <c r="A3" s="55"/>
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="65" t="s">
+      <c r="C3" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
       <c r="F3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="65"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="61"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="53"/>
       <c r="L3" s="5" t="s">
         <v>13</v>
       </c>
@@ -1502,7 +1481,7 @@
       <c r="J4" s="11">
         <v>101861</v>
       </c>
-      <c r="K4" s="42" t="s">
+      <c r="K4" s="34" t="s">
         <v>21</v>
       </c>
       <c r="L4" s="12" t="s">
@@ -1540,7 +1519,7 @@
       <c r="J5" s="11">
         <v>101862</v>
       </c>
-      <c r="K5" s="43" t="s">
+      <c r="K5" s="35" t="s">
         <v>21</v>
       </c>
       <c r="L5" s="12" t="s">
@@ -1576,7 +1555,7 @@
       <c r="J6" s="11">
         <v>101865</v>
       </c>
-      <c r="K6" s="43" t="s">
+      <c r="K6" s="35" t="s">
         <v>33</v>
       </c>
       <c r="L6" s="12" t="s">
@@ -1614,7 +1593,7 @@
       <c r="J7" s="11">
         <v>102531</v>
       </c>
-      <c r="K7" s="44" t="s">
+      <c r="K7" s="36" t="s">
         <v>39</v>
       </c>
       <c r="L7" s="12" t="s">
@@ -1643,7 +1622,7 @@
       </c>
       <c r="I8" s="20"/>
       <c r="J8" s="20"/>
-      <c r="K8" s="45"/>
+      <c r="K8" s="37"/>
       <c r="L8" s="20"/>
     </row>
     <row r="9" spans="1:14" ht="57" x14ac:dyDescent="0.25">
@@ -1677,7 +1656,7 @@
       <c r="J9" s="11">
         <v>102533</v>
       </c>
-      <c r="K9" s="44" t="s">
+      <c r="K9" s="36" t="s">
         <v>46</v>
       </c>
       <c r="L9" s="12" t="s">
@@ -1715,7 +1694,7 @@
       <c r="J10" s="11">
         <v>102534</v>
       </c>
-      <c r="K10" s="44" t="s">
+      <c r="K10" s="36" t="s">
         <v>51</v>
       </c>
       <c r="L10" s="12" t="s">
@@ -1753,7 +1732,7 @@
       <c r="J11" s="11">
         <v>103521</v>
       </c>
-      <c r="K11" s="44" t="s">
+      <c r="K11" s="36" t="s">
         <v>58</v>
       </c>
       <c r="L11" s="12" t="s">
@@ -1791,7 +1770,7 @@
       <c r="J12" s="11">
         <v>103522</v>
       </c>
-      <c r="K12" s="44" t="s">
+      <c r="K12" s="36" t="s">
         <v>62</v>
       </c>
       <c r="L12" s="12" t="s">
@@ -1829,7 +1808,7 @@
       <c r="J13" s="11">
         <v>103523</v>
       </c>
-      <c r="K13" s="44" t="s">
+      <c r="K13" s="36" t="s">
         <v>69</v>
       </c>
       <c r="L13" s="12" t="s">
@@ -1867,7 +1846,7 @@
       <c r="J14" s="11">
         <v>103524</v>
       </c>
-      <c r="K14" s="44" t="s">
+      <c r="K14" s="36" t="s">
         <v>73</v>
       </c>
       <c r="L14" s="12" t="s">
@@ -1905,7 +1884,7 @@
       <c r="J15" s="11">
         <v>104521</v>
       </c>
-      <c r="K15" s="44" t="s">
+      <c r="K15" s="36" t="s">
         <v>78</v>
       </c>
       <c r="L15" s="12" t="s">
@@ -1943,7 +1922,7 @@
       <c r="J16" s="11">
         <v>104522</v>
       </c>
-      <c r="K16" s="44" t="s">
+      <c r="K16" s="36" t="s">
         <v>85</v>
       </c>
       <c r="L16" s="12" t="s">
@@ -1981,7 +1960,7 @@
       <c r="J17" s="11">
         <v>104523</v>
       </c>
-      <c r="K17" s="44" t="s">
+      <c r="K17" s="36" t="s">
         <v>90</v>
       </c>
       <c r="L17" s="12" t="s">
@@ -2019,7 +1998,7 @@
       <c r="J18" s="11">
         <v>105521</v>
       </c>
-      <c r="K18" s="44" t="s">
+      <c r="K18" s="36" t="s">
         <v>95</v>
       </c>
       <c r="L18" s="12" t="s">
@@ -2055,7 +2034,7 @@
       <c r="J19" s="11">
         <v>105522</v>
       </c>
-      <c r="K19" s="46" t="s">
+      <c r="K19" s="38" t="s">
         <v>100</v>
       </c>
       <c r="L19" s="12" t="s">
@@ -2091,7 +2070,7 @@
       <c r="J20" s="11">
         <v>106521</v>
       </c>
-      <c r="K20" s="46" t="s">
+      <c r="K20" s="38" t="s">
         <v>104</v>
       </c>
       <c r="L20" s="12" t="s">
@@ -2127,7 +2106,7 @@
       <c r="J21" s="11">
         <v>107521</v>
       </c>
-      <c r="K21" s="46" t="s">
+      <c r="K21" s="38" t="s">
         <v>109</v>
       </c>
       <c r="L21" s="12" t="s">
@@ -2165,7 +2144,7 @@
       <c r="J22" s="11">
         <v>108521</v>
       </c>
-      <c r="K22" s="46" t="s">
+      <c r="K22" s="38" t="s">
         <v>115</v>
       </c>
       <c r="L22" s="12" t="s">
@@ -2173,83 +2152,83 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="40" t="s">
+      <c r="A23" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="B23" s="52" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="52" t="s">
+      <c r="B23" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="D23" s="53"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="52" t="s">
+      <c r="D23" s="44"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="G23" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="H23" s="52" t="s">
+      <c r="G23" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="H23" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="I23" s="55">
+      <c r="I23" s="46">
         <v>7290019570820</v>
       </c>
-      <c r="J23" s="56">
+      <c r="J23" s="47">
         <v>108523</v>
       </c>
-      <c r="K23" s="51" t="s">
+      <c r="K23" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="L23" s="57" t="s">
+      <c r="L23" s="48" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="40" t="s">
+      <c r="A24" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="B24" s="70" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="52" t="s">
+      <c r="B24" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="43" t="s">
         <v>121</v>
       </c>
-      <c r="D24" s="53"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="52" t="s">
+      <c r="D24" s="44"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="G24" s="52"/>
-      <c r="H24" s="52" t="s">
+      <c r="G24" s="43"/>
+      <c r="H24" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="I24" s="55">
+      <c r="I24" s="46">
         <v>7290019570820</v>
       </c>
-      <c r="J24" s="56">
+      <c r="J24" s="47">
         <v>188521</v>
       </c>
-      <c r="K24" s="51" t="s">
+      <c r="K24" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="L24" s="57" t="s">
+      <c r="L24" s="48" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="57" x14ac:dyDescent="0.25">
-      <c r="A25" s="40" t="s">
+      <c r="A25" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="26" t="s">
         <v>24</v>
       </c>
       <c r="C25" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="D25" s="31"/>
-      <c r="E25" s="32" t="s">
+      <c r="D25" s="27"/>
+      <c r="E25" s="28" t="s">
         <v>127</v>
       </c>
       <c r="F25" s="14" t="s">
@@ -2261,13 +2240,13 @@
       <c r="H25" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="I25" s="33">
+      <c r="I25" s="29">
         <v>7290019570813</v>
       </c>
       <c r="J25" s="11">
         <v>108522</v>
       </c>
-      <c r="K25" s="48" t="s">
+      <c r="K25" s="39" t="s">
         <v>129</v>
       </c>
       <c r="L25" s="12" t="s">
@@ -2275,19 +2254,19 @@
       </c>
     </row>
     <row r="26" spans="1:12" ht="57" x14ac:dyDescent="0.25">
-      <c r="A26" s="34" t="s">
+      <c r="A26" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="B26" s="30" t="s">
+      <c r="B26" s="26" t="s">
         <v>24</v>
       </c>
       <c r="C26" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="D26" s="35" t="s">
+      <c r="D26" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="E26" s="32" t="s">
+      <c r="E26" s="28" t="s">
         <v>133</v>
       </c>
       <c r="F26" s="14" t="s">
@@ -2299,13 +2278,13 @@
       <c r="H26" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="I26" s="33">
+      <c r="I26" s="29">
         <v>7290019570806</v>
       </c>
       <c r="J26" s="11">
         <v>110531</v>
       </c>
-      <c r="K26" s="49" t="s">
+      <c r="K26" s="40" t="s">
         <v>135</v>
       </c>
       <c r="L26" s="12" t="s">
@@ -2343,7 +2322,7 @@
       <c r="J27" s="11">
         <v>110532</v>
       </c>
-      <c r="K27" s="44" t="s">
+      <c r="K27" s="36" t="s">
         <v>140</v>
       </c>
       <c r="L27" s="12" t="s">
@@ -2381,7 +2360,7 @@
       <c r="J28" s="11">
         <v>110533</v>
       </c>
-      <c r="K28" s="44" t="s">
+      <c r="K28" s="36" t="s">
         <v>146</v>
       </c>
       <c r="L28" s="12" t="s">
@@ -2417,44 +2396,44 @@
       <c r="J29" s="11">
         <v>170521</v>
       </c>
-      <c r="K29" s="46" t="s">
+      <c r="K29" s="38" t="s">
         <v>151</v>
       </c>
       <c r="L29" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A30" s="36" t="s">
+    <row r="30" spans="1:12" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="62" t="s">
         <v>152</v>
       </c>
-      <c r="B30" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="C30" s="26" t="s">
+      <c r="B30" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="43" t="s">
         <v>153</v>
       </c>
-      <c r="D30" s="37"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="26" t="s">
+      <c r="D30" s="63"/>
+      <c r="E30" s="64"/>
+      <c r="F30" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="G30" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="H30" s="39" t="s">
+      <c r="G30" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="H30" s="65" t="s">
         <v>154</v>
       </c>
-      <c r="I30" s="27">
+      <c r="I30" s="46">
         <v>7290019570783</v>
       </c>
-      <c r="J30" s="28">
+      <c r="J30" s="47">
         <v>170522</v>
       </c>
-      <c r="K30" s="47" t="s">
+      <c r="K30" s="42" t="s">
         <v>155</v>
       </c>
-      <c r="L30" s="29" t="s">
+      <c r="L30" s="48" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2489,7 +2468,7 @@
       <c r="J31" s="11">
         <v>109521</v>
       </c>
-      <c r="K31" s="50" t="s">
+      <c r="K31" s="41" t="s">
         <v>160</v>
       </c>
       <c r="L31" s="12" t="s">
@@ -2525,7 +2504,7 @@
       <c r="J32" s="11">
         <v>109522</v>
       </c>
-      <c r="K32" s="46" t="s">
+      <c r="K32" s="38" t="s">
         <v>164</v>
       </c>
       <c r="L32" s="12" t="s">
@@ -2561,7 +2540,7 @@
       <c r="J33" s="11">
         <v>109523</v>
       </c>
-      <c r="K33" s="46" t="s">
+      <c r="K33" s="38" t="s">
         <v>168</v>
       </c>
       <c r="L33" s="12" t="s">
@@ -2595,7 +2574,7 @@
       <c r="J34" s="11">
         <v>157521</v>
       </c>
-      <c r="K34" s="46" t="s">
+      <c r="K34" s="38" t="s">
         <v>172</v>
       </c>
       <c r="L34" s="12" t="s">
@@ -2631,7 +2610,7 @@
       <c r="J35" s="11">
         <v>109524</v>
       </c>
-      <c r="K35" s="46" t="s">
+      <c r="K35" s="38" t="s">
         <v>177</v>
       </c>
       <c r="L35" s="12" t="s">
@@ -2663,7 +2642,7 @@
       <c r="J36" s="11">
         <v>109525</v>
       </c>
-      <c r="K36" s="48" t="s">
+      <c r="K36" s="39" t="s">
         <v>179</v>
       </c>
       <c r="L36" s="12" t="s">
@@ -2697,7 +2676,7 @@
       <c r="J37" s="11">
         <v>155521</v>
       </c>
-      <c r="K37" s="50" t="s">
+      <c r="K37" s="41" t="s">
         <v>185</v>
       </c>
       <c r="L37" s="12" t="s">
@@ -2731,7 +2710,7 @@
       <c r="J38" s="11">
         <v>153521</v>
       </c>
-      <c r="K38" s="46" t="s">
+      <c r="K38" s="38" t="s">
         <v>189</v>
       </c>
       <c r="L38" s="12" t="s">
@@ -2765,7 +2744,7 @@
       <c r="J39" s="11">
         <v>150521</v>
       </c>
-      <c r="K39" s="46" t="s">
+      <c r="K39" s="38" t="s">
         <v>193</v>
       </c>
       <c r="L39" s="12" t="s">
@@ -2801,7 +2780,7 @@
       <c r="J40" s="11">
         <v>151521</v>
       </c>
-      <c r="K40" s="44" t="s">
+      <c r="K40" s="36" t="s">
         <v>196</v>
       </c>
       <c r="L40" s="12" t="s">
@@ -2837,7 +2816,7 @@
       <c r="J41" s="11">
         <v>156521</v>
       </c>
-      <c r="K41" s="48" t="s">
+      <c r="K41" s="39" t="s">
         <v>200</v>
       </c>
       <c r="L41" s="12" t="s">

</xml_diff>

<commit_message>
cambio de img hebreo a etiqueta 308-he brazuelo con hueso - jabat
</commit_message>
<xml_diff>
--- a/jabad def.xlsx
+++ b/jabad def.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07303E88-A29C-40BA-9075-6ADF202B32FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A03C2B-7D65-4782-843D-5F0E4068A9D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1039,6 +1039,18 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1074,18 +1086,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1371,8 +1371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1386,37 +1386,37 @@
     <col min="8" max="8" width="13.5703125" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="121.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="151.7109375" customWidth="1"/>
     <col min="12" max="12" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="58" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1"/>
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="58" t="s">
+      <c r="D2" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="58" t="s">
+      <c r="E2" s="62" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="56" t="s">
+      <c r="H2" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="60" t="s">
+      <c r="I2" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="50" t="s">
+      <c r="J2" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="52" t="s">
+      <c r="K2" s="56" t="s">
         <v>7</v>
       </c>
       <c r="L2" s="3" t="s">
@@ -1427,25 +1427,25 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="55"/>
+      <c r="A3" s="59"/>
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="57" t="s">
+      <c r="C3" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
       <c r="F3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="57"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="53"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="57"/>
       <c r="L3" s="5" t="s">
         <v>13</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="57" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="32" t="s">
         <v>125</v>
       </c>
@@ -2246,7 +2246,7 @@
       <c r="J25" s="11">
         <v>108522</v>
       </c>
-      <c r="K25" s="39" t="s">
+      <c r="K25" s="42" t="s">
         <v>129</v>
       </c>
       <c r="L25" s="12" t="s">
@@ -2404,7 +2404,7 @@
       </c>
     </row>
     <row r="30" spans="1:12" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="62" t="s">
+      <c r="A30" s="50" t="s">
         <v>152</v>
       </c>
       <c r="B30" s="43" t="s">
@@ -2413,15 +2413,15 @@
       <c r="C30" s="43" t="s">
         <v>153</v>
       </c>
-      <c r="D30" s="63"/>
-      <c r="E30" s="64"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="52"/>
       <c r="F30" s="43" t="s">
         <v>18</v>
       </c>
       <c r="G30" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="H30" s="65" t="s">
+      <c r="H30" s="53" t="s">
         <v>154</v>
       </c>
       <c r="I30" s="46">

</xml_diff>

<commit_message>
cambio de img hebreo a etiqueta 182- he-asado sh 9c 99 - jabat
</commit_message>
<xml_diff>
--- a/jabad def.xlsx
+++ b/jabad def.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A03C2B-7D65-4782-843D-5F0E4068A9D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A83D846B-8080-4EC7-8469-2818CFD5D456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -896,7 +896,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1086,6 +1086,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1371,8 +1374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -2437,7 +2440,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="114" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="22">
         <v>99</v>
       </c>
@@ -2468,7 +2471,7 @@
       <c r="J31" s="11">
         <v>109521</v>
       </c>
-      <c r="K31" s="41" t="s">
+      <c r="K31" s="66" t="s">
         <v>160</v>
       </c>
       <c r="L31" s="12" t="s">

</xml_diff>

<commit_message>
cambio de img hebreo a etiqueta 187-he-entrecostilla ch- jabat
</commit_message>
<xml_diff>
--- a/jabad def.xlsx
+++ b/jabad def.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A83D846B-8080-4EC7-8469-2818CFD5D456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E04EEB9-090E-4063-94FD-115DB988893E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1051,6 +1051,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1086,9 +1089,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1374,8 +1374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1395,31 +1395,31 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="59" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1"/>
-      <c r="C2" s="60" t="s">
+      <c r="C2" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="62" t="s">
+      <c r="D2" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="62" t="s">
+      <c r="E2" s="63" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="60" t="s">
+      <c r="H2" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="64" t="s">
+      <c r="I2" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="54" t="s">
+      <c r="J2" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="56" t="s">
+      <c r="K2" s="57" t="s">
         <v>7</v>
       </c>
       <c r="L2" s="3" t="s">
@@ -1430,25 +1430,25 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="59"/>
+      <c r="A3" s="60"/>
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="61" t="s">
+      <c r="C3" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
       <c r="F3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="61"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="57"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="58"/>
       <c r="L3" s="5" t="s">
         <v>13</v>
       </c>
@@ -2471,7 +2471,7 @@
       <c r="J31" s="11">
         <v>109521</v>
       </c>
-      <c r="K31" s="66" t="s">
+      <c r="K31" s="54" t="s">
         <v>160</v>
       </c>
       <c r="L31" s="12" t="s">
@@ -2620,7 +2620,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="57" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="17"/>
       <c r="B36" s="14" t="s">
         <v>24</v>
@@ -2645,7 +2645,7 @@
       <c r="J36" s="11">
         <v>109525</v>
       </c>
-      <c r="K36" s="39" t="s">
+      <c r="K36" s="42" t="s">
         <v>179</v>
       </c>
       <c r="L36" s="12" t="s">

</xml_diff>

<commit_message>
cambio de img hebreo a etiqueta 162-he-molleja - jabat
</commit_message>
<xml_diff>
--- a/jabad def.xlsx
+++ b/jabad def.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Santa Giulia\ETIQUETAS\INTERNAS\HEBREO\JABAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{526AA06A-E181-4210-A31B-C8009FA01F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{445B88F5-7E77-4245-AE9E-5CF5BD2D383F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -896,7 +896,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1004,9 +1004,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" readingOrder="2"/>
     </xf>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1371,8 +1368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1392,31 +1389,31 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="57" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1"/>
-      <c r="C2" s="60" t="s">
+      <c r="C2" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="62" t="s">
+      <c r="D2" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="62" t="s">
+      <c r="E2" s="61" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="60" t="s">
+      <c r="H2" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="64" t="s">
+      <c r="I2" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="54" t="s">
+      <c r="J2" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="56" t="s">
+      <c r="K2" s="55" t="s">
         <v>7</v>
       </c>
       <c r="L2" s="3" t="s">
@@ -1427,25 +1424,25 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="59"/>
+      <c r="A3" s="58"/>
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="61" t="s">
+      <c r="C3" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
       <c r="F3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="61"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="57"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="56"/>
       <c r="L3" s="5" t="s">
         <v>13</v>
       </c>
@@ -2155,33 +2152,33 @@
       <c r="A23" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="B23" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="42" t="s">
+      <c r="B23" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="41" t="s">
         <v>117</v>
       </c>
-      <c r="D23" s="43"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="42" t="s">
+      <c r="D23" s="42"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="G23" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="H23" s="42" t="s">
+      <c r="G23" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="H23" s="41" t="s">
         <v>118</v>
       </c>
-      <c r="I23" s="45">
+      <c r="I23" s="44">
         <v>7290019570820</v>
       </c>
-      <c r="J23" s="46">
+      <c r="J23" s="45">
         <v>108523</v>
       </c>
-      <c r="K23" s="41" t="s">
+      <c r="K23" s="40" t="s">
         <v>119</v>
       </c>
-      <c r="L23" s="47" t="s">
+      <c r="L23" s="46" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2189,31 +2186,31 @@
       <c r="A24" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="B24" s="48" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="42" t="s">
+      <c r="B24" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="41" t="s">
         <v>121</v>
       </c>
-      <c r="D24" s="43"/>
-      <c r="E24" s="44"/>
-      <c r="F24" s="42" t="s">
+      <c r="D24" s="42"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42" t="s">
+      <c r="G24" s="41"/>
+      <c r="H24" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="I24" s="45">
+      <c r="I24" s="44">
         <v>7290019570820</v>
       </c>
-      <c r="J24" s="46">
+      <c r="J24" s="45">
         <v>188521</v>
       </c>
-      <c r="K24" s="41" t="s">
+      <c r="K24" s="40" t="s">
         <v>124</v>
       </c>
-      <c r="L24" s="47" t="s">
+      <c r="L24" s="46" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2246,7 +2243,7 @@
       <c r="J25" s="11">
         <v>108522</v>
       </c>
-      <c r="K25" s="41" t="s">
+      <c r="K25" s="40" t="s">
         <v>129</v>
       </c>
       <c r="L25" s="12" t="s">
@@ -2284,7 +2281,7 @@
       <c r="J26" s="11">
         <v>110531</v>
       </c>
-      <c r="K26" s="40" t="s">
+      <c r="K26" s="39" t="s">
         <v>135</v>
       </c>
       <c r="L26" s="12" t="s">
@@ -2404,36 +2401,36 @@
       </c>
     </row>
     <row r="30" spans="1:12" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="49" t="s">
+      <c r="A30" s="48" t="s">
         <v>152</v>
       </c>
-      <c r="B30" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="C30" s="42" t="s">
+      <c r="B30" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="41" t="s">
         <v>153</v>
       </c>
-      <c r="D30" s="50"/>
-      <c r="E30" s="51"/>
-      <c r="F30" s="42" t="s">
+      <c r="D30" s="49"/>
+      <c r="E30" s="50"/>
+      <c r="F30" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="G30" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="H30" s="52" t="s">
+      <c r="G30" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="H30" s="51" t="s">
         <v>154</v>
       </c>
-      <c r="I30" s="45">
+      <c r="I30" s="44">
         <v>7290019570783</v>
       </c>
-      <c r="J30" s="46">
+      <c r="J30" s="45">
         <v>170522</v>
       </c>
-      <c r="K30" s="41" t="s">
+      <c r="K30" s="40" t="s">
         <v>155</v>
       </c>
-      <c r="L30" s="47" t="s">
+      <c r="L30" s="46" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2468,7 +2465,7 @@
       <c r="J31" s="11">
         <v>109521</v>
       </c>
-      <c r="K31" s="53" t="s">
+      <c r="K31" s="52" t="s">
         <v>160</v>
       </c>
       <c r="L31" s="12" t="s">
@@ -2642,7 +2639,7 @@
       <c r="J36" s="11">
         <v>109525</v>
       </c>
-      <c r="K36" s="41" t="s">
+      <c r="K36" s="40" t="s">
         <v>179</v>
       </c>
       <c r="L36" s="12" t="s">
@@ -2676,7 +2673,7 @@
       <c r="J37" s="11">
         <v>155521</v>
       </c>
-      <c r="K37" s="53" t="s">
+      <c r="K37" s="52" t="s">
         <v>185</v>
       </c>
       <c r="L37" s="12" t="s">
@@ -2787,7 +2784,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="57" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="17"/>
       <c r="B41" s="14" t="s">
         <v>24</v>
@@ -2816,7 +2813,7 @@
       <c r="J41" s="11">
         <v>156521</v>
       </c>
-      <c r="K41" s="39" t="s">
+      <c r="K41" s="40" t="s">
         <v>200</v>
       </c>
       <c r="L41" s="12" t="s">

</xml_diff>